<commit_message>
Se agregaron desagregaciones del INPC subyacente y no subyacente en la automatización de la descarga de las series.
</commit_message>
<xml_diff>
--- a/data/inpc_api.xlsx
+++ b/data/inpc_api.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,7 +426,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>INPC CCM</t>
+          <t>Subyacente - Mercancias</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -436,19 +436,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>e|865543</t>
+          <t>e|865548</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>v_inpc_ccm</t>
+          <t>v_subyacente_mercancias</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>No subyacente</t>
+          <t>Subyacente - Servicios</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -458,173 +458,173 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>e|865555</t>
+          <t>e|865551</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>v_inpc_nsubyacente</t>
+          <t>v_subyacente_servicios</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>INPC quincenal</t>
+          <t>INPC CCM</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>112001600020</t>
+          <t>112001700010</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>e|821890</t>
+          <t>e|865543</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>v_inpc_quincenal</t>
+          <t>v_inpc_ccm</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INPC quincenal subyacente</t>
+          <t>No subyacente</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>112001600020</t>
+          <t>112001700010</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>e|821891</t>
+          <t>e|865555</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>v_subyacente_quincenal</t>
+          <t>v_inpc_nsubyacente</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>INPC quincenal nsubyacente</t>
+          <t>No subyacente - Agropecuarios</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>112001600020</t>
+          <t>112001700010</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>e|821901</t>
+          <t>e|865556</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>v_nsubyacente_quincenal</t>
+          <t>v_nsubyacente_agropecuarios</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tortilla</t>
+          <t>No subyacente - Energéticos y tarifas autorizadas</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>112001700030</t>
+          <t>112001700010</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>e|865594</t>
+          <t>e|865559</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>v_tortilla</t>
+          <t>v_nsubyacente_energeticos</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Huevo</t>
+          <t>INPC quincenal</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>112001700030</t>
+          <t>112001600020</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>e|865663</t>
+          <t>e|821890</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>v_huevo</t>
+          <t>v_inpc_quincenal</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Leche</t>
+          <t>INPC quincenal subyacente</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>112001700030</t>
+          <t>112001600020</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>e|865647</t>
+          <t>e|821891</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>v_leche</t>
+          <t>v_subyacente_quincenal</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carne res</t>
+          <t>INPC quincenal nsubyacente</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>112001700030</t>
+          <t>112001600020</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>e|865625</t>
+          <t>e|821901</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>v_carne_res</t>
+          <t>v_nsubyacente_quincenal</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Frijol</t>
+          <t>Tortilla</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -634,1374 +634,1462 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>e|865706</t>
+          <t>e|865594</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>v_frijol</t>
+          <t>v_tortilla</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>INPP sin petróleo</t>
+          <t>Huevo</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>112001900050</t>
+          <t>112001700030</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>e|1700001</t>
+          <t>e|865663</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>v_inpp</t>
+          <t>v_huevo</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>INPP primarias</t>
+          <t>Leche</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>112001900050</t>
+          <t>112001700030</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>e|1700003</t>
+          <t>e|865647</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>v_inpp_primarias</t>
+          <t>v_leche</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>INPP secundarias sin petróleo</t>
+          <t>Carne res</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>112001900050</t>
+          <t>112001700030</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>e|1700160</t>
+          <t>e|865625</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>v_inpp_secundarias</t>
+          <t>v_carne_res</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>INPP terciarias</t>
+          <t>Frijol</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>112001900050</t>
+          <t>112001700030</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>e|1701070</t>
+          <t>e|865706</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>v_inpp_terciarias</t>
+          <t>v_frijol</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>INPP finales</t>
+          <t>INPP sin petróleo</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1120019000300020</t>
+          <t>112001900050</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>e|1380005</t>
+          <t>e|1700001</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>v_inpp_finales</t>
+          <t>v_inpp</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>INPP intermedios</t>
+          <t>INPP primarias</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1120019000400010</t>
+          <t>112001900050</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>e|1750002</t>
+          <t>e|1700003</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>v_inpp_intermedios</t>
+          <t>v_inpp_primarias</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Área Met. de la CDMX</t>
+          <t>INPP secundarias sin petróleo</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1120017000600010</t>
+          <t>112001900050</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>e|870982</t>
+          <t>e|1700160</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>v_ciudad_870982</t>
+          <t>v_inpp_secundarias</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Acapulco, Gro.</t>
+          <t>INPP terciarias</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1120017000600020</t>
+          <t>112001900050</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>e|871518</t>
+          <t>e|1701070</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>v_ciudad_871518</t>
+          <t>v_inpp_terciarias</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Aguascalientes, Ags.</t>
+          <t>INPP finales</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1120017000600030</t>
+          <t>1120019000300020</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>e|871948</t>
+          <t>e|1380005</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>v_ciudad_871948</t>
+          <t>v_inpp_finales</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Atlacomulco, Méx.</t>
+          <t>INPP intermedios</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1120017000600040</t>
+          <t>1120019000400010</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>e|872378</t>
+          <t>e|1750002</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>v_ciudad_872378</t>
+          <t>v_inpp_intermedios</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Campeche, Camp.</t>
+          <t>Área Met. de la CDMX</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1120017000600050</t>
+          <t>1120017000600010</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>e|872808</t>
+          <t>e|870982</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>v_ciudad_872808</t>
+          <t>v_ciudad_870982</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cancún, Q. Roo.</t>
+          <t>Acapulco, Gro.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1120017000600060</t>
+          <t>1120017000600020</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>e|873238</t>
+          <t>e|871518</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>v_ciudad_873238</t>
+          <t>v_ciudad_871518</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Cd. Acuña, Coah.</t>
+          <t>Aguascalientes, Ags.</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1120017000600070</t>
+          <t>1120017000600030</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>e|873668</t>
+          <t>e|871948</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>v_ciudad_873668</t>
+          <t>v_ciudad_871948</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Cd. Jiménez, Chih.</t>
+          <t>Atlacomulco, Méx.</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1120017000600080</t>
+          <t>1120017000600040</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>e|874098</t>
+          <t>e|872378</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>v_ciudad_874098</t>
+          <t>v_ciudad_872378</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Cd. Juárez, Chih.</t>
+          <t>Campeche, Camp.</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1120017000600090</t>
+          <t>1120017000600050</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>e|874528</t>
+          <t>e|872808</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>v_ciudad_874528</t>
+          <t>v_ciudad_872808</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Chetumal, Q.R.</t>
+          <t>Cancún, Q. Roo.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1120017000600100</t>
+          <t>1120017000600060</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>e|874958</t>
+          <t>e|873238</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>v_ciudad_876248</t>
+          <t>v_ciudad_873238</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Chihuahua, Chih.</t>
+          <t>Cd. Acuña, Coah.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1120017000600110</t>
+          <t>1120017000600070</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>e|875388</t>
+          <t>e|873668</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>v_ciudad_876678</t>
+          <t>v_ciudad_873668</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Coatzacoalcos, Ver.</t>
+          <t>Cd. Jiménez, Chih.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1120017000600120</t>
+          <t>1120017000600080</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>e|875818</t>
+          <t>e|874098</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>v_ciudad_877108</t>
+          <t>v_ciudad_874098</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Colima, Col.</t>
+          <t>Cd. Juárez, Chih.</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1120017000600130</t>
+          <t>1120017000600090</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>e|876248</t>
+          <t>e|874528</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>v_ciudad_877538</t>
+          <t>v_ciudad_874528</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Córdoba, Ver.</t>
+          <t>Chetumal, Q.R.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1120017000600140</t>
+          <t>1120017000600100</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>e|876678</t>
+          <t>e|874958</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>v_ciudad_877968</t>
+          <t>v_ciudad_876248</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Cortazar, Gto.</t>
+          <t>Chihuahua, Chih.</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1120017000600150</t>
+          <t>1120017000600110</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>e|877108</t>
+          <t>e|875388</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>v_ciudad_874958</t>
+          <t>v_ciudad_876678</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Cuernavaca, Mor.</t>
+          <t>Coatzacoalcos, Ver.</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1120017000600160</t>
+          <t>1120017000600120</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>e|877538</t>
+          <t>e|875818</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>v_ciudad_875388</t>
+          <t>v_ciudad_877108</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Culiacán, Sin.</t>
+          <t>Colima, Col.</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1120017000600170</t>
+          <t>1120017000600130</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>e|877968</t>
+          <t>e|876248</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>v_ciudad_875818</t>
+          <t>v_ciudad_877538</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Durango, Dgo.</t>
+          <t>Córdoba, Ver.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1120017000600180</t>
+          <t>1120017000600140</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>e|878398</t>
+          <t>e|876678</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>v_ciudad_878398</t>
+          <t>v_ciudad_877968</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Esperanza, Son.</t>
+          <t>Cortazar, Gto.</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1120017000600190</t>
+          <t>1120017000600150</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>e|878828</t>
+          <t>e|877108</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>v_ciudad_878828</t>
+          <t>v_ciudad_874958</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Fresnillo, Zac.</t>
+          <t>Cuernavaca, Mor.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1120017000600200</t>
+          <t>1120017000600160</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>e|879258</t>
+          <t>e|877538</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>v_ciudad_879258</t>
+          <t>v_ciudad_875388</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Guadalajara, Jal.</t>
+          <t>Culiacán, Sin.</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1120017000600210</t>
+          <t>1120017000600170</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>e|879688</t>
+          <t>e|877968</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>v_ciudad_879688</t>
+          <t>v_ciudad_875818</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Hermosillo, Son.</t>
+          <t>Durango, Dgo.</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1120017000600220</t>
+          <t>1120017000600180</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>e|880224</t>
+          <t>e|878398</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>v_ciudad_880224</t>
+          <t>v_ciudad_878398</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Huatabampo, Son.</t>
+          <t>Esperanza, Son.</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1120017000600230</t>
+          <t>1120017000600190</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>e|880654</t>
+          <t>e|878828</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>v_ciudad_880654</t>
+          <t>v_ciudad_878828</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Iguala, Gro.</t>
+          <t>Fresnillo, Zac.</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1120017000600240</t>
+          <t>1120017000600200</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>e|881084</t>
+          <t>e|879258</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>v_ciudad_881084</t>
+          <t>v_ciudad_879258</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Izúcar de Matamoros, Pue.</t>
+          <t>Guadalajara, Jal.</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>1120017000600250</t>
+          <t>1120017000600210</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>e|881514</t>
+          <t>e|879688</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>v_ciudad_881514</t>
+          <t>v_ciudad_879688</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Jacona, Mich.</t>
+          <t>Hermosillo, Son.</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1120017000600260</t>
+          <t>1120017000600220</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>e|881944</t>
+          <t>e|880224</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>v_ciudad_881944</t>
+          <t>v_ciudad_880224</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>La Paz, B.C.S.</t>
+          <t>Huatabampo, Son.</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1120017000600270</t>
+          <t>1120017000600230</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>e|882374</t>
+          <t>e|880654</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>v_ciudad_882374</t>
+          <t>v_ciudad_880654</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>León, Gto.</t>
+          <t>Iguala, Gro.</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1120017000600280</t>
+          <t>1120017000600240</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>e|882804</t>
+          <t>e|881084</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>v_ciudad_882804</t>
+          <t>v_ciudad_881084</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Matamoros, Tamps.</t>
+          <t>Izúcar de Matamoros, Pue.</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1120017000600290</t>
+          <t>1120017000600250</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>e|883234</t>
+          <t>e|881514</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>v_ciudad_883234</t>
+          <t>v_ciudad_881514</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mérida, Yuc.</t>
+          <t>Jacona, Mich.</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1120017000600300</t>
+          <t>1120017000600260</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>e|883664</t>
+          <t>e|881944</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>v_ciudad_883664</t>
+          <t>v_ciudad_881944</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Mexicali, B.C.</t>
+          <t>La Paz, B.C.S.</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>1120017000600310</t>
+          <t>1120017000600270</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>e|884094</t>
+          <t>e|882374</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>v_ciudad_884094</t>
+          <t>v_ciudad_882374</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Monclova, Coah.</t>
+          <t>León, Gto.</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1120017000600320</t>
+          <t>1120017000600280</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>e|884524</t>
+          <t>e|882804</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>v_ciudad_884524</t>
+          <t>v_ciudad_882804</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Monterrey, N.L.</t>
+          <t>Matamoros, Tamps.</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1120017000600330</t>
+          <t>1120017000600290</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>e|884954</t>
+          <t>e|883234</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>v_ciudad_884954</t>
+          <t>v_ciudad_883234</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Morelia, Mich.</t>
+          <t>Mérida, Yuc.</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1120017000600340</t>
+          <t>1120017000600300</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>e|885490</t>
+          <t>e|883664</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>v_ciudad_885490</t>
+          <t>v_ciudad_883664</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Oaxaca, Oax.</t>
+          <t>Mexicali, B.C.</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1120017000600350</t>
+          <t>1120017000600310</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>e|885920</t>
+          <t>e|884094</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>v_ciudad_885920</t>
+          <t>v_ciudad_884094</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Pachuca, Hgo.</t>
+          <t>Monclova, Coah.</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1120017000600360</t>
+          <t>1120017000600320</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>e|886350</t>
+          <t>e|884524</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>v_ciudad_886350</t>
+          <t>v_ciudad_884524</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Puebla, Pue.</t>
+          <t>Monterrey, N.L.</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1120017000600370</t>
+          <t>1120017000600330</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>e|886780</t>
+          <t>e|884954</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>v_ciudad_886780</t>
+          <t>v_ciudad_884954</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Querétaro, Qro.</t>
+          <t>Morelia, Mich.</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1120017000600380</t>
+          <t>1120017000600340</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>e|887210</t>
+          <t>e|885490</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>v_ciudad_887210</t>
+          <t>v_ciudad_885490</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Saltillo, Coah.</t>
+          <t>Oaxaca, Oax.</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1120017000600390</t>
+          <t>1120017000600350</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>e|887640</t>
+          <t>e|885920</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>v_ciudad_887640</t>
+          <t>v_ciudad_885920</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>San Andrés Tuxtla, Ver.</t>
+          <t>Pachuca, Hgo.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>1120017000600400</t>
+          <t>1120017000600360</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>e|888070</t>
+          <t>e|886350</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>v_ciudad_888070</t>
+          <t>v_ciudad_886350</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>San Luis Potosí, S.L.P.</t>
+          <t>Puebla, Pue.</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1120017000600410</t>
+          <t>1120017000600370</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>e|888500</t>
+          <t>e|886780</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>v_ciudad_888500</t>
+          <t>v_ciudad_886780</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Tampico, Tamps.</t>
+          <t>Querétaro, Qro.</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1120017000600420</t>
+          <t>1120017000600380</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>e|888930</t>
+          <t>e|887210</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>v_ciudad_888930</t>
+          <t>v_ciudad_887210</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Tapachula, Chis.</t>
+          <t>Saltillo, Coah.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>1120017000600430</t>
+          <t>1120017000600390</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>e|889360</t>
+          <t>e|887640</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>v_ciudad_889360</t>
+          <t>v_ciudad_887640</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Tehuantepec, Oax.</t>
+          <t>San Andrés Tuxtla, Ver.</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1120017000600440</t>
+          <t>1120017000600400</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>e|889790</t>
+          <t>e|888070</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>v_ciudad_889790</t>
+          <t>v_ciudad_888070</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Tepatitlán, Jal.</t>
+          <t>San Luis Potosí, S.L.P.</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1120017000600450</t>
+          <t>1120017000600410</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>e|890220</t>
+          <t>e|888500</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>v_ciudad_890220</t>
+          <t>v_ciudad_888500</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Tepic, Nay.</t>
+          <t>Tampico, Tamps.</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1120017000600460</t>
+          <t>1120017000600420</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>e|890650</t>
+          <t>e|888930</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>v_ciudad_890650</t>
+          <t>v_ciudad_888930</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Tijuana, B.C.</t>
+          <t>Tapachula, Chis.</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>1120017000600470</t>
+          <t>1120017000600430</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>e|891080</t>
+          <t>e|889360</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>v_ciudad_891080</t>
+          <t>v_ciudad_889360</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Tlaxcala, Tlax.</t>
+          <t>Tehuantepec, Oax.</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1120017000600480</t>
+          <t>1120017000600440</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>e|891510</t>
+          <t>e|889790</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>v_ciudad_891510</t>
+          <t>v_ciudad_889790</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Toluca, Edo. de Méx.</t>
+          <t>Tepatitlán, Jal.</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>1120017000600490</t>
+          <t>1120017000600450</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>e|891940</t>
+          <t>e|890220</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>v_ciudad_891940</t>
+          <t>v_ciudad_890220</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Torreón, Coah.</t>
+          <t>Tepic, Nay.</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>1120017000600500</t>
+          <t>1120017000600460</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>e|892370</t>
+          <t>e|890650</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>v_ciudad_892370</t>
+          <t>v_ciudad_890650</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Tulancingo, Hgo.</t>
+          <t>Tijuana, B.C.</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>1120017000600510</t>
+          <t>1120017000600470</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>e|892800</t>
+          <t>e|891080</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>v_ciudad_892800</t>
+          <t>v_ciudad_891080</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Tuxtla Gutiérrez, Chis.</t>
+          <t>Tlaxcala, Tlax.</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>1120017000600520</t>
+          <t>1120017000600480</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>e|893230</t>
+          <t>e|891510</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>v_ciudad_893230</t>
+          <t>v_ciudad_891510</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Veracruz, Ver.</t>
+          <t>Toluca, Edo. de Méx.</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>1120017000600530</t>
+          <t>1120017000600490</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>e|893660</t>
+          <t>e|891940</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>v_ciudad_893660</t>
+          <t>v_ciudad_891940</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Villahermosa, Tab.</t>
+          <t>Torreón, Coah.</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1120017000600540</t>
+          <t>1120017000600500</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>e|894090</t>
+          <t>e|892370</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>v_ciudad_894090</t>
+          <t>v_ciudad_892370</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Zacatecas, Zac.</t>
+          <t>Tulancingo, Hgo.</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>1120017000600550</t>
+          <t>1120017000600510</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>e|894520</t>
+          <t>e|892800</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>v_ciudad_894520</t>
+          <t>v_ciudad_892800</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>Tuxtla Gutiérrez, Chis.</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>1120017000600520</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>e|893230</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>v_ciudad_893230</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Veracruz, Ver.</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>1120017000600530</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>e|893660</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>v_ciudad_893660</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Villahermosa, Tab.</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1120017000600540</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>e|894090</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>v_ciudad_894090</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Zacatecas, Zac.</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1120017000600550</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>e|894520</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>v_ciudad_894520</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
           <t>Nacional</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="B79" t="inlineStr">
         <is>
           <t>112001700010</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>e|865541</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>v_ciudad_inpc</t>
         </is>

</xml_diff>